<commit_message>
added important notes and connection to SQlite DB
</commit_message>
<xml_diff>
--- a/aCCTg. pROGRAm/fs 2015.xlsx
+++ b/aCCTg. pROGRAm/fs 2015.xlsx
@@ -736,10 +736,10 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2759,167 +2759,167 @@
         <f t="shared" ref="C19:AR19" si="1">SUM(C7:C18)</f>
         <v>1736465.7799999998</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="41">
         <f t="shared" si="1"/>
         <v>97738.5</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="41">
         <f t="shared" si="1"/>
         <v>14950</v>
       </c>
-      <c r="F19" s="42">
+      <c r="F19" s="41">
         <f t="shared" si="1"/>
         <v>1915</v>
       </c>
-      <c r="G19" s="42">
+      <c r="G19" s="41">
         <f t="shared" si="1"/>
         <v>46566.13</v>
       </c>
-      <c r="H19" s="42">
+      <c r="H19" s="41">
         <f t="shared" si="1"/>
         <v>346977.55</v>
       </c>
-      <c r="I19" s="42">
+      <c r="I19" s="41">
         <f t="shared" si="1"/>
         <v>2960</v>
       </c>
-      <c r="J19" s="42">
+      <c r="J19" s="41">
         <f t="shared" si="1"/>
         <v>6000</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="41">
         <f t="shared" si="1"/>
         <v>2550</v>
       </c>
-      <c r="L19" s="42">
+      <c r="L19" s="41">
         <f t="shared" si="1"/>
         <v>1299</v>
       </c>
-      <c r="M19" s="42">
+      <c r="M19" s="41">
         <f t="shared" si="1"/>
         <v>4004</v>
       </c>
-      <c r="N19" s="42">
+      <c r="N19" s="41">
         <f t="shared" si="1"/>
         <v>3300</v>
       </c>
-      <c r="O19" s="42">
+      <c r="O19" s="41">
         <f t="shared" si="1"/>
         <v>867337.36999999988</v>
       </c>
-      <c r="P19" s="42">
+      <c r="P19" s="41">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="Q19" s="42">
+      <c r="Q19" s="41">
         <f t="shared" si="1"/>
         <v>554</v>
       </c>
-      <c r="R19" s="42">
+      <c r="R19" s="41">
         <f t="shared" si="1"/>
         <v>32342.6</v>
       </c>
-      <c r="S19" s="42">
+      <c r="S19" s="41">
         <f t="shared" si="1"/>
         <v>64960</v>
       </c>
-      <c r="T19" s="42">
+      <c r="T19" s="41">
         <f t="shared" si="1"/>
         <v>39036</v>
       </c>
-      <c r="U19" s="42">
+      <c r="U19" s="41">
         <f t="shared" si="1"/>
         <v>16333</v>
       </c>
-      <c r="V19" s="42">
+      <c r="V19" s="41">
         <f t="shared" si="1"/>
         <v>-36814.99</v>
       </c>
-      <c r="W19" s="42">
+      <c r="W19" s="41">
         <f t="shared" si="1"/>
         <v>-12832</v>
       </c>
-      <c r="X19" s="42">
+      <c r="X19" s="41">
         <f t="shared" si="1"/>
         <v>2831.83</v>
       </c>
-      <c r="Y19" s="42">
+      <c r="Y19" s="41">
         <f t="shared" si="1"/>
         <v>39096.5</v>
       </c>
-      <c r="Z19" s="42">
+      <c r="Z19" s="41">
         <f t="shared" si="1"/>
         <v>7256</v>
       </c>
-      <c r="AA19" s="42">
+      <c r="AA19" s="41">
         <f t="shared" si="1"/>
         <v>1918</v>
       </c>
-      <c r="AB19" s="42">
+      <c r="AB19" s="41">
         <f t="shared" si="1"/>
         <v>9188.8799999999992</v>
       </c>
-      <c r="AC19" s="42">
+      <c r="AC19" s="41">
         <f t="shared" si="1"/>
         <v>2356</v>
       </c>
-      <c r="AD19" s="42">
+      <c r="AD19" s="41">
         <f t="shared" si="1"/>
         <v>1980</v>
       </c>
-      <c r="AE19" s="42">
+      <c r="AE19" s="41">
         <f t="shared" si="1"/>
         <v>54394</v>
       </c>
-      <c r="AF19" s="42">
+      <c r="AF19" s="41">
         <f t="shared" si="1"/>
         <v>3713</v>
       </c>
-      <c r="AG19" s="42">
+      <c r="AG19" s="41">
         <f t="shared" si="1"/>
         <v>5533</v>
       </c>
-      <c r="AH19" s="42">
+      <c r="AH19" s="41">
         <f t="shared" si="1"/>
         <v>37665</v>
       </c>
-      <c r="AI19" s="42">
+      <c r="AI19" s="41">
         <f t="shared" si="1"/>
         <v>322.7</v>
       </c>
-      <c r="AJ19" s="42">
+      <c r="AJ19" s="41">
         <f t="shared" si="1"/>
         <v>-57444.290000000023</v>
       </c>
-      <c r="AK19" s="42">
+      <c r="AK19" s="41">
         <f t="shared" si="1"/>
         <v>47340</v>
       </c>
-      <c r="AL19" s="42">
+      <c r="AL19" s="41">
         <f t="shared" si="1"/>
         <v>26755</v>
       </c>
-      <c r="AM19" s="42">
+      <c r="AM19" s="41">
         <f t="shared" si="1"/>
         <v>2231</v>
       </c>
-      <c r="AN19" s="42">
+      <c r="AN19" s="41">
         <f t="shared" si="1"/>
         <v>1300</v>
       </c>
-      <c r="AO19" s="42">
+      <c r="AO19" s="41">
         <f t="shared" si="1"/>
         <v>18400</v>
       </c>
-      <c r="AP19" s="42">
+      <c r="AP19" s="41">
         <f t="shared" si="1"/>
         <v>24840</v>
       </c>
-      <c r="AQ19" s="42">
+      <c r="AQ19" s="41">
         <f t="shared" si="1"/>
         <v>4600</v>
       </c>
-      <c r="AR19" s="42">
+      <c r="AR19" s="41">
         <f t="shared" si="1"/>
         <v>2713</v>
       </c>
@@ -3031,10 +3031,10 @@
   <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C83" sqref="C83"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3090,26 +3090,26 @@
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41" t="s">
+      <c r="E3" s="42"/>
+      <c r="F3" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41" t="s">
+      <c r="I3" s="42"/>
+      <c r="J3" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41" t="s">
+      <c r="K3" s="42"/>
+      <c r="L3" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="M3" s="41"/>
+      <c r="M3" s="42"/>
     </row>
     <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">

</xml_diff>